<commit_message>
Taylor working on heartbeat
</commit_message>
<xml_diff>
--- a/a5/ResultsCompiled.xlsx
+++ b/a5/ResultsCompiled.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25540" windowHeight="14220" tabRatio="500"/>
+    <workbookView xWindow="1820" yWindow="1140" windowWidth="25540" windowHeight="14220" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="correct" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="PieContig" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="33">
   <si>
     <t>Hypothesis of Ranking</t>
   </si>
@@ -306,8 +307,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,7 +419,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -445,6 +448,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -473,6 +477,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -804,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -12580,8 +12585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N151"/>
   <sheetViews>
-    <sheetView topLeftCell="I2" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="N39" sqref="A1:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17380,4 +17385,1266 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2.192017369063028</v>
+      </c>
+      <c r="E2">
+        <v>85.55556</v>
+      </c>
+      <c r="F2">
+        <v>90</v>
+      </c>
+      <c r="G2">
+        <f xml:space="preserve"> SUM(D2:D39)</f>
+        <v>102.17060483248984</v>
+      </c>
+      <c r="H2">
+        <f xml:space="preserve"> G2/38</f>
+        <v>2.6887001271707853</v>
+      </c>
+      <c r="I2">
+        <f xml:space="preserve"> D2 - H2</f>
+        <v>-0.49668275810775731</v>
+      </c>
+      <c r="J2">
+        <f xml:space="preserve"> POWER(I2,2)</f>
+        <v>0.24669376220152894</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> SUM(J2:J39)</f>
+        <v>78.271945733038351</v>
+      </c>
+      <c r="L2">
+        <f>K2/38</f>
+        <v>2.0597880456062723</v>
+      </c>
+      <c r="M2" s="8">
+        <f xml:space="preserve"> SQRT(L2)</f>
+        <v>1.4351961697295155</v>
+      </c>
+      <c r="N2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1.0213105739378452</v>
+      </c>
+      <c r="E3">
+        <v>61.904761999999998</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>2.6887001271707853</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I39" si="0" xml:space="preserve"> D3 - H3</f>
+        <v>-1.6673895532329401</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J39" si="1" xml:space="preserve"> POWER(I3,2)</f>
+        <v>2.7801879222303438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.26534087321696426</v>
+      </c>
+      <c r="E4">
+        <v>98.076920000000001</v>
+      </c>
+      <c r="F4">
+        <v>97</v>
+      </c>
+      <c r="H4">
+        <v>2.6887001271707853</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>-2.4233592539538211</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>5.8726700737236204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>-0.19264507794239591</v>
+      </c>
+      <c r="E5" s="7">
+        <v>86.25</v>
+      </c>
+      <c r="F5" s="7">
+        <v>87</v>
+      </c>
+      <c r="H5">
+        <v>2.6887001271707853</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>-2.8813452051131812</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>8.3021501910287192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>2.9241226948681929</v>
+      </c>
+      <c r="E6" s="7">
+        <v>89.534880000000001</v>
+      </c>
+      <c r="F6" s="7">
+        <v>97</v>
+      </c>
+      <c r="H6">
+        <v>2.6887001271707853</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.23542256769740755</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>5.5423785381240438E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>4.4298552108167826</v>
+      </c>
+      <c r="E7" s="7">
+        <v>51.428573999999998</v>
+      </c>
+      <c r="F7" s="7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>2.6887001271707853</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>1.7411550836459972</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>3.0316210253062996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0.54431721863138038</v>
+      </c>
+      <c r="E8">
+        <v>83.333330000000004</v>
+      </c>
+      <c r="F8">
+        <v>82</v>
+      </c>
+      <c r="H8">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>-2.1443829085394097</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>4.5983780584359382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>1.6048636391936544</v>
+      </c>
+      <c r="E9">
+        <v>97.916669999999996</v>
+      </c>
+      <c r="F9">
+        <v>95</v>
+      </c>
+      <c r="H9">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>-1.0838364879771358</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>1.1747015326706121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>4.701210244421449</v>
+      </c>
+      <c r="E10" s="7">
+        <v>58.888890000000004</v>
+      </c>
+      <c r="F10" s="7">
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>2.0125101172506588</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>4.0501969720362601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1.0874628412503395</v>
+      </c>
+      <c r="E11" s="7">
+        <v>50</v>
+      </c>
+      <c r="F11" s="7">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>-1.6012372859204507</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>2.563960845821891</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>3.1523838245250104</v>
+      </c>
+      <c r="E12" s="7">
+        <v>33.766235000000002</v>
+      </c>
+      <c r="F12" s="7">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.46368369735422021</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0.21500257119208008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>3.0839672879238482</v>
+      </c>
+      <c r="E13" s="7">
+        <v>68.354429999999994</v>
+      </c>
+      <c r="F13" s="7">
+        <v>60</v>
+      </c>
+      <c r="H13">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.39526716075305801</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0.15623612836978382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>2.5255452387852597</v>
+      </c>
+      <c r="E14">
+        <v>50.632910000000003</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+      <c r="H14">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>-0.16315488838553049</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>2.6619517604094912E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1.7982330440737391</v>
+      </c>
+      <c r="E15">
+        <v>82.352940000000004</v>
+      </c>
+      <c r="F15">
+        <v>79</v>
+      </c>
+      <c r="H15">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>-0.89046708309705114</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0.79293162607937062</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>-0.48755261673906297</v>
+      </c>
+      <c r="E16">
+        <v>95.588234</v>
+      </c>
+      <c r="F16">
+        <v>95</v>
+      </c>
+      <c r="H16">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>-3.1762527439098531</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>10.088581493194871</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>4.2093361516433303</v>
+      </c>
+      <c r="E17">
+        <v>43.373497</v>
+      </c>
+      <c r="F17">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>1.5206360244725401</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>2.3123339189236516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="7">
+        <v>14</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>1.7900780430648904</v>
+      </c>
+      <c r="E18" s="7">
+        <v>93.333336000000003</v>
+      </c>
+      <c r="F18" s="7">
+        <v>90</v>
+      </c>
+      <c r="H18">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>-0.89862208410589983</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0.80752165004283094</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="7">
+        <v>15</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>3.2735839200462582</v>
+      </c>
+      <c r="E19" s="7">
+        <v>70.454543999999999</v>
+      </c>
+      <c r="F19" s="7">
+        <v>80</v>
+      </c>
+      <c r="H19">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.58488379287546799</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>0.34208905116839333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="7">
+        <v>16</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>4.3200141007348822</v>
+      </c>
+      <c r="E20" s="7">
+        <v>34.848483999999999</v>
+      </c>
+      <c r="F20" s="7">
+        <v>15</v>
+      </c>
+      <c r="H20">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>1.631313973564092</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>2.661185280345467</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="7">
+        <v>17</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>2.8207508201945122</v>
+      </c>
+      <c r="E21" s="7">
+        <v>88.059700000000007</v>
+      </c>
+      <c r="F21" s="7">
+        <v>95</v>
+      </c>
+      <c r="H21">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0.13205069302372197</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>1.7437385528045253E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="7">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>2.0609518117552508</v>
+      </c>
+      <c r="E22" s="7">
+        <v>94.047614999999993</v>
+      </c>
+      <c r="F22" s="7">
+        <v>90</v>
+      </c>
+      <c r="H22">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>-0.62774831541553944</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>0.3940679475070476</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="7">
+        <v>18</v>
+      </c>
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>4.41981324714558</v>
+      </c>
+      <c r="E23" s="7">
+        <v>66.279070000000004</v>
+      </c>
+      <c r="F23" s="7">
+        <v>45</v>
+      </c>
+      <c r="H23">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>1.7311131199747898</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>2.9967526341488511</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="7">
+        <v>18</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>3.4514032825003387</v>
+      </c>
+      <c r="E24" s="7">
+        <v>55.813957000000002</v>
+      </c>
+      <c r="F24" s="7">
+        <v>45</v>
+      </c>
+      <c r="H24">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0.76270315532954847</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0.58171610314964939</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="7">
+        <v>19</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>2.2527850056281156</v>
+      </c>
+      <c r="E25" s="7">
+        <v>74.358980000000003</v>
+      </c>
+      <c r="F25" s="7">
+        <v>79</v>
+      </c>
+      <c r="H25">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>-0.43591512154267464</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0.19002199318956481</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="7">
+        <v>20</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>4.3309168781146168</v>
+      </c>
+      <c r="E26" s="7">
+        <v>80</v>
+      </c>
+      <c r="F26" s="7">
+        <v>60</v>
+      </c>
+      <c r="H26">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>1.6422167509438266</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>2.696875857080498</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>3.173656431295107</v>
+      </c>
+      <c r="E27">
+        <v>33.898308</v>
+      </c>
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="H27">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0.48495630412431678</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0.23518261690991682</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>3.4881152046722148</v>
+      </c>
+      <c r="E28">
+        <v>41.095889999999997</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="H28">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0.7994150775014246</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.63906446613660872</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="7">
+        <v>22</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>4.4334774822129033</v>
+      </c>
+      <c r="E29" s="7">
+        <v>34.482757999999997</v>
+      </c>
+      <c r="F29" s="7">
+        <v>13</v>
+      </c>
+      <c r="H29">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>1.7447773550421131</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>3.0442480186677519</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="7">
+        <v>23</v>
+      </c>
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>0.97607763479859966</v>
+      </c>
+      <c r="E30" s="7">
+        <v>88.157889999999995</v>
+      </c>
+      <c r="F30" s="7">
+        <v>90</v>
+      </c>
+      <c r="H30">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>-1.7126224923721907</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>2.9330758013791343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="7">
+        <v>24</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>2.9582970385156813</v>
+      </c>
+      <c r="E31" s="7">
+        <v>82.352940000000004</v>
+      </c>
+      <c r="F31" s="7">
+        <v>90</v>
+      </c>
+      <c r="H31">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>0.26959691134489105</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>7.2682494606705048E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="7">
+        <v>25</v>
+      </c>
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>3.5532416665752846</v>
+      </c>
+      <c r="E32" s="7">
+        <v>45.614032999999999</v>
+      </c>
+      <c r="F32" s="7">
+        <v>34</v>
+      </c>
+      <c r="H32">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>0.86454153940449441</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>0.74743207335589301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="7">
+        <v>26</v>
+      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>5.3113697820811172</v>
+      </c>
+      <c r="E33" s="7">
+        <v>89.583330000000004</v>
+      </c>
+      <c r="F33" s="7">
+        <v>50</v>
+      </c>
+      <c r="H33">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>2.622669654910327</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>6.878396118787454</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="7">
+        <v>26</v>
+      </c>
+      <c r="B34" s="7">
+        <v>2</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>1.1572119069372728</v>
+      </c>
+      <c r="E34" s="7">
+        <v>92.105260000000001</v>
+      </c>
+      <c r="F34" s="7">
+        <v>90</v>
+      </c>
+      <c r="H34">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>-1.5314882202335174</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>2.3454561687140267</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="7">
+        <v>27</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>4.4738023643407789</v>
+      </c>
+      <c r="E35" s="7">
+        <v>61.904761999999998</v>
+      </c>
+      <c r="F35" s="7">
+        <v>84</v>
+      </c>
+      <c r="H35">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>1.7851022371699887</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>3.1865899971492988</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="7">
+        <v>28</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>2.7049494076636953</v>
+      </c>
+      <c r="E36" s="7">
+        <v>31.395350000000001</v>
+      </c>
+      <c r="F36" s="7">
+        <v>25</v>
+      </c>
+      <c r="H36">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>1.6249280492905083E-2</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>2.6403911653710563E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="7">
+        <v>29</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>2.1410109077174444</v>
+      </c>
+      <c r="E37" s="7">
+        <v>85.714290000000005</v>
+      </c>
+      <c r="F37" s="7">
+        <v>90</v>
+      </c>
+      <c r="H37">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>-0.54768921945334581</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>0.29996348110541521</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="7">
+        <v>29</v>
+      </c>
+      <c r="B38" s="7">
+        <v>2</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>2.5712360472413791</v>
+      </c>
+      <c r="E38" s="7">
+        <v>68.181815999999998</v>
+      </c>
+      <c r="F38" s="7">
+        <v>74</v>
+      </c>
+      <c r="H38">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>-0.1174640799294111</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>1.379781007366308E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="7">
+        <v>30</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>3.6480933315845472</v>
+      </c>
+      <c r="E39" s="7">
+        <v>70.588234</v>
+      </c>
+      <c r="F39" s="7">
+        <v>83</v>
+      </c>
+      <c r="H39">
+        <v>2.6887001271707902</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>0.95939320441375697</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>0.92043532067529688</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>